<commit_message>
Change the computations of the KPIs
</commit_message>
<xml_diff>
--- a/Instances/01_Lumpy.xlsx
+++ b/Instances/01_Lumpy.xlsx
@@ -842,13 +842,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1465</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0.026</v>
       </c>
       <c r="E2" t="n">
-        <v>7.004406089811704</v>
+        <v>15.496</v>
       </c>
       <c r="F2" t="n">
         <v>0.26</v>
@@ -871,13 +871,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>584</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0248</v>
       </c>
       <c r="E3" t="n">
-        <v>3.175340471132494</v>
+        <v>5.952000000000001</v>
       </c>
       <c r="F3" t="n">
         <v>0.248</v>
@@ -900,13 +900,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>2060</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0.0048</v>
       </c>
       <c r="E4" t="n">
-        <v>2.022862283020591</v>
+        <v>4.0128</v>
       </c>
       <c r="F4" t="n">
         <v>0.048</v>
@@ -929,13 +929,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>2060</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0.002</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7707994952412393</v>
+        <v>1.672</v>
       </c>
       <c r="F5" t="n">
         <v>0.02</v>
@@ -958,13 +958,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2060</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0036</v>
       </c>
       <c r="E6" t="n">
-        <v>1.59318261338783</v>
+        <v>3.0096</v>
       </c>
       <c r="F6" t="n">
         <v>0.036</v>
@@ -987,13 +987,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1242</v>
+        <v>3796</v>
       </c>
       <c r="D7" t="n">
         <v>0.026</v>
       </c>
       <c r="E7" t="n">
-        <v>6.80884064404836</v>
+        <v>13.156</v>
       </c>
       <c r="F7" t="n">
         <v>0.26</v>
@@ -1016,13 +1016,13 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>216</v>
+        <v>676</v>
       </c>
       <c r="D8" t="n">
         <v>0.0508</v>
       </c>
       <c r="E8" t="n">
-        <v>1.967185363589409</v>
+        <v>4.572</v>
       </c>
       <c r="F8" t="n">
         <v>0.508</v>
@@ -1045,13 +1045,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>363</v>
+        <v>1126</v>
       </c>
       <c r="D9" t="n">
         <v>0.0248</v>
       </c>
       <c r="E9" t="n">
-        <v>1.924393602442972</v>
+        <v>3.72</v>
       </c>
       <c r="F9" t="n">
         <v>0.248</v>
@@ -1533,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1072.8</v>
+        <v>8940</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1541,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>432</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1549,7 +1549,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2257.2</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1557,7 +1557,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2257.2</v>
+        <v>20900</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1565,7 +1565,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1504.8</v>
+        <v>20900</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1573,7 +1573,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1821.6</v>
+        <v>7590</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1581,7 +1581,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>405</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1589,7 +1589,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>540</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +1642,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1706,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1866,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>